<commit_message>
Generalização tabela LateX ok.
</commit_message>
<xml_diff>
--- a/dados/rgt_paineis_covid.xlsx
+++ b/dados/rgt_paineis_covid.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="base" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sem_acentos" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve">Brasil.io</t>
   </si>
@@ -104,6 +105,54 @@
   </si>
   <si>
     <t xml:space="preserve">Tabela clara de casos/UF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confiavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desagradavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agradavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difícil de encontrar a informacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facil encontrar a informaca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difícil navegacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graficos mais modernos, facil navegacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muita navegacao para conseguir as informacoes solicitadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graficos simples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informacao detalhada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informacao rapida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Painel e rapido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obscuridade na proveniencia dos dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clareza na proveniencia dos dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta de confianca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confianca</t>
   </si>
 </sst>
 </file>
@@ -326,14 +375,14 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.54"/>
   </cols>
@@ -8503,4 +8552,293 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.05"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>